<commit_message>
Fix issues in measurements (re-measured the mass)
</commit_message>
<xml_diff>
--- a/0-data/0-raw/tree1h.xlsx
+++ b/0-data/0-raw/tree1h.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$N$1:$N$1184</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$K$1:$K$1184</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1139" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I1185" sqref="I1185"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8827,7 +8827,7 @@
         <v>-0.19489999999999999</v>
       </c>
       <c r="S453">
-        <v>9.0920000000000005</v>
+        <v>1.5780000000000001</v>
       </c>
     </row>
     <row r="454" spans="1:19" x14ac:dyDescent="0.3">
@@ -9176,7 +9176,7 @@
         <v>-0.27110000000000001</v>
       </c>
       <c r="S468">
-        <v>9.0429999999999993</v>
+        <v>2.54</v>
       </c>
     </row>
     <row r="469" spans="1:19" x14ac:dyDescent="0.3">
@@ -23887,8 +23887,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D817E2E441AD8840AD152F485CF91FFD" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="9bd92fc451d28d7a43c1e2d68c8f297e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3bb3ef3-874e-4bfe-a810-81c575a8e62c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6122410798bbeb3d5138414ef9c1dd21" ns2:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D817E2E441AD8840AD152F485CF91FFD" ma:contentTypeVersion="6" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="66b1d846b1b9efb7ee546c90ee14313c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3bb3ef3-874e-4bfe-a810-81c575a8e62c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f185daa67cb9aaba26ea2e5f6e3f3c05" ns2:_="">
     <xsd:import namespace="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -23898,6 +23907,10 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -23916,6 +23929,28 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -24018,15 +24053,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -24034,24 +24060,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EB56767-F5A8-48F9-B0FC-4412AF94E6A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B02E33F-DE6E-4C32-8CFE-5083680231C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -24059,18 +24067,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A70317-2E0F-429B-BA37-3DCDF25D9859}"/>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{594950B9-4EE5-490F-9C8F-74E6C5FB1587}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>